<commit_message>
title style and  rp total is ok.
</commit_message>
<xml_diff>
--- a/QueryReport/excelTemplate/Employee_template1_20200303120000.xlsx
+++ b/QueryReport/excelTemplate/Employee_template1_20200303120000.xlsx
@@ -302,8 +302,15 @@
     <x:numFmt numFmtId="240" formatCode="yyyy-mm-dd"/>
     <x:numFmt numFmtId="240" formatCode="yyyy-mm-dd"/>
     <x:numFmt numFmtId="240" formatCode="yyyy-mm-dd"/>
+    <x:numFmt numFmtId="240" formatCode="yyyy-mm-dd"/>
+    <x:numFmt numFmtId="240" formatCode="yyyy-mm-dd"/>
+    <x:numFmt numFmtId="240" formatCode="yyyy-mm-dd"/>
+    <x:numFmt numFmtId="240" formatCode="yyyy-mm-dd"/>
+    <x:numFmt numFmtId="240" formatCode="yyyy-mm-dd"/>
+    <x:numFmt numFmtId="240" formatCode="yyyy-mm-dd"/>
+    <x:numFmt numFmtId="240" formatCode="yyyy-mm-dd"/>
   </x:numFmts>
-  <x:fonts count="22">
+  <x:fonts count="36">
     <x:font>
       <x:sz val="11"/>
       <x:color rgb="FF000000"/>
@@ -328,6 +335,83 @@
       <x:name val="Microsoft YaHei"/>
       <x:family val="2"/>
       <x:charset val="134"/>
+    </x:font>
+    <x:font>
+      <x:name val="Microsoft YaHei"/>
+      <x:sz val="11"/>
+      <x:color rgb="000000"/>
+    </x:font>
+    <x:font>
+      <x:name val="Microsoft YaHei"/>
+      <x:sz val="11"/>
+      <x:b/>
+      <x:color rgb="000000"/>
+    </x:font>
+    <x:font>
+      <x:name val="Microsoft YaHei"/>
+      <x:sz val="11"/>
+      <x:color rgb="000000"/>
+    </x:font>
+    <x:font>
+      <x:name val="Microsoft YaHei"/>
+      <x:sz val="11"/>
+      <x:b/>
+      <x:color rgb="000000"/>
+    </x:font>
+    <x:font>
+      <x:name val="Microsoft YaHei"/>
+      <x:sz val="11"/>
+      <x:color rgb="000000"/>
+    </x:font>
+    <x:font>
+      <x:name val="Microsoft YaHei"/>
+      <x:sz val="11"/>
+      <x:b/>
+      <x:color rgb="000000"/>
+    </x:font>
+    <x:font>
+      <x:name val="Microsoft YaHei"/>
+      <x:sz val="11"/>
+      <x:color rgb="000000"/>
+    </x:font>
+    <x:font>
+      <x:name val="Microsoft YaHei"/>
+      <x:sz val="11"/>
+      <x:b/>
+      <x:color rgb="000000"/>
+    </x:font>
+    <x:font>
+      <x:name val="Microsoft YaHei"/>
+      <x:sz val="11"/>
+      <x:color rgb="000000"/>
+    </x:font>
+    <x:font>
+      <x:name val="Microsoft YaHei"/>
+      <x:sz val="11"/>
+      <x:b/>
+      <x:color rgb="000000"/>
+    </x:font>
+    <x:font>
+      <x:name val="Microsoft YaHei"/>
+      <x:sz val="11"/>
+      <x:color rgb="000000"/>
+    </x:font>
+    <x:font>
+      <x:name val="Microsoft YaHei"/>
+      <x:sz val="11"/>
+      <x:b/>
+      <x:color rgb="000000"/>
+    </x:font>
+    <x:font>
+      <x:name val="Microsoft YaHei"/>
+      <x:sz val="11"/>
+      <x:color rgb="000000"/>
+    </x:font>
+    <x:font>
+      <x:name val="Microsoft YaHei"/>
+      <x:sz val="11"/>
+      <x:b/>
+      <x:color rgb="000000"/>
     </x:font>
     <x:font>
       <x:name val="Microsoft YaHei"/>
@@ -457,7 +541,7 @@
       <x:alignment vertical="center"/>
     </x:xf>
   </x:cellStyleXfs>
-  <x:cellXfs count="34">
+  <x:cellXfs count="55">
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <x:alignment vertical="center"/>
     </x:xf>
@@ -504,6 +588,27 @@
     <x:xf fontId="20" borderId="0" applyFont="1"/>
     <x:xf fontId="21" borderId="0" applyFont="1"/>
     <x:xf numFmtId="240" fontId="20" borderId="0" applyNumberFormat="1" applyFont="1"/>
+    <x:xf fontId="22" borderId="0" applyFont="1"/>
+    <x:xf fontId="23" borderId="0" applyFont="1"/>
+    <x:xf numFmtId="240" fontId="22" borderId="0" applyNumberFormat="1" applyFont="1"/>
+    <x:xf fontId="24" borderId="0" applyFont="1"/>
+    <x:xf fontId="25" borderId="0" applyFont="1"/>
+    <x:xf numFmtId="240" fontId="24" borderId="0" applyNumberFormat="1" applyFont="1"/>
+    <x:xf fontId="26" borderId="0" applyFont="1"/>
+    <x:xf fontId="27" borderId="0" applyFont="1"/>
+    <x:xf numFmtId="240" fontId="26" borderId="0" applyNumberFormat="1" applyFont="1"/>
+    <x:xf fontId="28" borderId="0" applyFont="1"/>
+    <x:xf fontId="29" borderId="0" applyFont="1"/>
+    <x:xf numFmtId="240" fontId="28" borderId="0" applyNumberFormat="1" applyFont="1"/>
+    <x:xf fontId="30" borderId="0" applyFont="1"/>
+    <x:xf fontId="31" borderId="0" applyFont="1"/>
+    <x:xf numFmtId="240" fontId="30" borderId="0" applyNumberFormat="1" applyFont="1"/>
+    <x:xf fontId="32" borderId="0" applyFont="1"/>
+    <x:xf fontId="33" borderId="0" applyFont="1"/>
+    <x:xf numFmtId="240" fontId="32" borderId="0" applyNumberFormat="1" applyFont="1"/>
+    <x:xf fontId="34" borderId="0" applyFont="1"/>
+    <x:xf fontId="35" borderId="0" applyFont="1"/>
+    <x:xf numFmtId="240" fontId="34" borderId="0" applyNumberFormat="1" applyFont="1"/>
   </x:cellXfs>
   <x:cellStyles count="1">
     <x:cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -524,7 +629,7 @@
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
 <x:pivotCacheDefinition xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" r:id="rId1" refreshOnLoad="1" refreshedBy="Administrator" refreshedDate="43893.643148263887" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="8" xr:uid="{CF51BC23-A1A6-4DE3-85A0-7D4C21EB6AB0}" mc:Ignorable="xr">
   <x:cacheSource type="worksheet">
-    <x:worksheetSource ref="B3:T19" sheet="Report"/>
+    <x:worksheetSource ref="B1:V17" sheet="Report"/>
   </x:cacheSource>
   <x:cacheFields count="21">
     <x:cacheField name="Contract Description" numFmtId="0">
@@ -1264,1028 +1369,1123 @@
   </x:sheetViews>
   <x:sheetFormatPr defaultRowHeight="14.25"/>
   <x:sheetData>
-    <x:row r="1" spans="1:20" ht="16.5">
-      <x:c r="C1" s="2" t="s">
-        <x:v>82</x:v>
+    <x:row r="1">
+      <x:c r="A1" s="52" t="str">
+        <x:v>_DATASTART</x:v>
+      </x:c>
+      <x:c r="B1" s="49" t="str">
+        <x:v>Contract Description</x:v>
+      </x:c>
+      <x:c r="C1" s="49" t="str">
+        <x:v>Staff Number</x:v>
+      </x:c>
+      <x:c r="D1" s="49" t="str">
+        <x:v>ename</x:v>
+      </x:c>
+      <x:c r="E1" s="49" t="str">
+        <x:v>Zone Name</x:v>
+      </x:c>
+      <x:c r="F1" s="49" t="str">
+        <x:v>Rank Name</x:v>
+      </x:c>
+      <x:c r="G1" s="49" t="str">
+        <x:v>Postition Code</x:v>
+      </x:c>
+      <x:c r="H1" s="49" t="str">
+        <x:v>p name ok 3</x:v>
+      </x:c>
+      <x:c r="I1" s="49" t="str">
+        <x:v>Join Date</x:v>
+      </x:c>
+      <x:c r="J1" s="49" t="str">
+        <x:v>Year of Service</x:v>
+      </x:c>
+      <x:c r="K1" s="49" t="str">
+        <x:v>Annual Leave Class</x:v>
+      </x:c>
+      <x:c r="L1" s="49" t="str">
+        <x:v>~!</x:v>
+      </x:c>
+      <x:c r="M1" s="49" t="str">
+        <x:v>Employment Type</x:v>
+      </x:c>
+      <x:c r="N1" s="49" t="str">
+        <x:v>Basic Salary</x:v>
+      </x:c>
+      <x:c r="O1" s="49" t="str">
+        <x:v>Pay Scale Point</x:v>
+      </x:c>
+      <x:c r="P1" s="49" t="str">
+        <x:v>PayScale Scheme</x:v>
+      </x:c>
+      <x:c r="Q1" s="49" t="str">
+        <x:v>Commence Date</x:v>
+      </x:c>
+      <x:c r="R1" s="49" t="str">
+        <x:v>Terminate Date</x:v>
+      </x:c>
+      <x:c r="S1" s="49" t="str">
+        <x:v>Staff Status</x:v>
+      </x:c>
+      <x:c r="T1" s="49" t="str">
+        <x:v>Part Time</x:v>
+      </x:c>
+      <x:c r="U1" s="49" t="str">
+        <x:v>SecurityGroupID</x:v>
+      </x:c>
+      <x:c r="V1" s="49" t="str">
+        <x:v>Securtiy Group</x:v>
       </x:c>
     </x:row>
-    <x:row r="2" spans="1:20" ht="16.5">
-      <x:c r="C2" s="3" t="s">
-        <x:v>81</x:v>
+    <x:row r="2">
+      <x:c r="B2" s="52" t="str">
+        <x:v>Data World Solutions Ltd</x:v>
+      </x:c>
+      <x:c r="C2" s="52" t="str">
+        <x:v>S31612</x:v>
+      </x:c>
+      <x:c r="D2" s="52" t="str">
+        <x:v>Chan Ka</x:v>
+      </x:c>
+      <x:c r="E2" s="52" t="str">
+        <x:v>Unit A</x:v>
+      </x:c>
+      <x:c r="F2" s="52" t="str">
+        <x:v>Assistant Manager 主管</x:v>
+      </x:c>
+      <x:c r="G2" s="52" t="str">
+        <x:v>OFFICER</x:v>
+      </x:c>
+      <x:c r="H2" s="52" t="str">
+        <x:v>OFFICER 主任</x:v>
+      </x:c>
+      <x:c r="I2" s="54" t="d">
+        <x:v>2016-01-01T00:00:00.0000000</x:v>
+      </x:c>
+      <x:c r="J2" s="52" t="n">
+        <x:v>4.224</x:v>
+      </x:c>
+      <x:c r="K2" s="52" t="str">
+        <x:v>AL14</x:v>
+      </x:c>
+      <x:c r="L2" s="52" t="str">
+        <x:v>Bank Holiday</x:v>
+      </x:c>
+      <x:c r="M2" s="52" t="str">
+        <x:v>Monthly</x:v>
+      </x:c>
+      <x:c r="N2" s="52" t="n">
+        <x:v>39554</x:v>
+      </x:c>
+      <x:c r="O2" s="52" t="n">
+        <x:v/>
+      </x:c>
+      <x:c r="P2" s="52" t="str">
+        <x:v/>
+      </x:c>
+      <x:c r="Q2" s="54" t="d">
+        <x:v>2016-04-01T00:00:00.0000000</x:v>
+      </x:c>
+      <x:c r="R2" s="54" t="d">
+        <x:v>2048-01-01T00:00:00.0000000</x:v>
+      </x:c>
+      <x:c r="S2" s="52" t="str">
+        <x:v>Active</x:v>
+      </x:c>
+      <x:c r="T2" s="52" t="str">
+        <x:v>No</x:v>
+      </x:c>
+      <x:c r="U2" s="52" t="n">
+        <x:v>39</x:v>
+      </x:c>
+      <x:c r="V2" s="52" t="str">
+        <x:v>DWS - CWB</x:v>
       </x:c>
     </x:row>
     <x:row r="3">
-      <x:c r="A3" s="31" t="str">
-        <x:v>_DATASTART</x:v>
-      </x:c>
-      <x:c r="B3" s="28" t="str">
-        <x:v>Contract Description</x:v>
-      </x:c>
-      <x:c r="C3" s="28" t="str">
-        <x:v>Staff Number</x:v>
-      </x:c>
-      <x:c r="D3" s="28" t="str">
-        <x:v>ename</x:v>
-      </x:c>
-      <x:c r="E3" s="28" t="str">
-        <x:v>Zone Name</x:v>
-      </x:c>
-      <x:c r="F3" s="28" t="str">
-        <x:v>p name ok 3</x:v>
-      </x:c>
-      <x:c r="G3" s="28" t="str">
-        <x:v>Join Date</x:v>
-      </x:c>
-      <x:c r="H3" s="28" t="str">
-        <x:v>Year of Service</x:v>
-      </x:c>
-      <x:c r="I3" s="28" t="str">
-        <x:v>Annual Leave Class</x:v>
-      </x:c>
-      <x:c r="J3" s="28" t="str">
-        <x:v>~!</x:v>
-      </x:c>
-      <x:c r="K3" s="28" t="str">
-        <x:v>Employment Type</x:v>
-      </x:c>
-      <x:c r="L3" s="28" t="str">
-        <x:v>Basic Salary</x:v>
-      </x:c>
-      <x:c r="M3" s="28" t="str">
-        <x:v>Pay Scale Point</x:v>
-      </x:c>
-      <x:c r="N3" s="28" t="str">
-        <x:v>PayScale Scheme</x:v>
-      </x:c>
-      <x:c r="O3" s="28" t="str">
-        <x:v>Commence Date</x:v>
-      </x:c>
-      <x:c r="P3" s="28" t="str">
-        <x:v>Terminate Date</x:v>
-      </x:c>
-      <x:c r="Q3" s="28" t="str">
-        <x:v>Staff Status</x:v>
-      </x:c>
-      <x:c r="R3" s="28" t="str">
-        <x:v>Part Time</x:v>
-      </x:c>
-      <x:c r="S3" s="28" t="str">
-        <x:v>SecurityGroupID</x:v>
-      </x:c>
-      <x:c r="T3" s="28" t="str">
-        <x:v>Securtiy Group</x:v>
+      <x:c r="B3" s="52" t="str">
+        <x:v>Data World Solutions Ltd</x:v>
+      </x:c>
+      <x:c r="C3" s="52" t="str">
+        <x:v>S31611</x:v>
+      </x:c>
+      <x:c r="D3" s="52" t="str">
+        <x:v>Chan Hang</x:v>
+      </x:c>
+      <x:c r="E3" s="52" t="str">
+        <x:v>Unit A</x:v>
+      </x:c>
+      <x:c r="F3" s="52" t="str">
+        <x:v>Assistant Manager 主管</x:v>
+      </x:c>
+      <x:c r="G3" s="52" t="str">
+        <x:v>SUPERVISOR</x:v>
+      </x:c>
+      <x:c r="H3" s="52" t="str">
+        <x:v>主任</x:v>
+      </x:c>
+      <x:c r="I3" s="54" t="d">
+        <x:v>2016-01-01T00:00:00.0000000</x:v>
+      </x:c>
+      <x:c r="J3" s="52" t="n">
+        <x:v>4.224</x:v>
+      </x:c>
+      <x:c r="K3" s="52" t="str">
+        <x:v>AL14</x:v>
+      </x:c>
+      <x:c r="L3" s="52" t="str">
+        <x:v>Bank Holiday</x:v>
+      </x:c>
+      <x:c r="M3" s="52" t="str">
+        <x:v>Monthly</x:v>
+      </x:c>
+      <x:c r="N3" s="52" t="n">
+        <x:v>30020</x:v>
+      </x:c>
+      <x:c r="O3" s="52" t="n">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="P3" s="52" t="str">
+        <x:v>MPS</x:v>
+      </x:c>
+      <x:c r="Q3" s="54" t="d">
+        <x:v>2016-04-01T00:00:00.0000000</x:v>
+      </x:c>
+      <x:c r="R3" s="54" t="d">
+        <x:v>2048-01-01T00:00:00.0000000</x:v>
+      </x:c>
+      <x:c r="S3" s="52" t="str">
+        <x:v>Active</x:v>
+      </x:c>
+      <x:c r="T3" s="52" t="str">
+        <x:v>No</x:v>
+      </x:c>
+      <x:c r="U3" s="52" t="n">
+        <x:v>39</x:v>
+      </x:c>
+      <x:c r="V3" s="52" t="str">
+        <x:v>DWS - CWB</x:v>
       </x:c>
     </x:row>
     <x:row r="4">
-      <x:c r="B4" s="31" t="str">
+      <x:c r="B4" s="52" t="str">
         <x:v>Data World Solutions Ltd</x:v>
       </x:c>
-      <x:c r="C4" s="31" t="str">
-        <x:v>AA100818</x:v>
-      </x:c>
-      <x:c r="D4" s="31" t="str">
-        <x:v>Chan Tai man 10</x:v>
-      </x:c>
-      <x:c r="E4" s="31" t="str">
+      <x:c r="C4" s="52" t="str">
+        <x:v>S30171</x:v>
+      </x:c>
+      <x:c r="D4" s="52" t="str">
+        <x:v>Chan Ka Man</x:v>
+      </x:c>
+      <x:c r="E4" s="52" t="str">
         <x:v>Unit A</x:v>
       </x:c>
-      <x:c r="F4" s="31" t="str">
-        <x:v>CARE WORKER 護理員</x:v>
-      </x:c>
-      <x:c r="G4" s="33" t="d">
-        <x:v>2019-10-11T00:00:00.0000000</x:v>
-      </x:c>
-      <x:c r="H4" s="31" t="n">
-        <x:v>0.4481</x:v>
-      </x:c>
-      <x:c r="I4" s="31" t="str">
-        <x:v>AL07</x:v>
-      </x:c>
-      <x:c r="J4" s="31" t="str">
-        <x:v>Bank Holiday</x:v>
-      </x:c>
-      <x:c r="K4" s="31" t="str">
+      <x:c r="F4" s="52" t="str">
+        <x:v>Assistant Manager 主管</x:v>
+      </x:c>
+      <x:c r="G4" s="52" t="str">
+        <x:v>SW</x:v>
+      </x:c>
+      <x:c r="H4" s="52" t="str">
+        <x:v>SOCIAL WORKER 社會工作員</x:v>
+      </x:c>
+      <x:c r="I4" s="54" t="d">
+        <x:v>2011-10-01T00:00:00.0000000</x:v>
+      </x:c>
+      <x:c r="J4" s="52" t="n">
+        <x:v>8.4781</x:v>
+      </x:c>
+      <x:c r="K4" s="52" t="str">
+        <x:v>AL10</x:v>
+      </x:c>
+      <x:c r="L4" s="52" t="str">
+        <x:v>Statutory Holiday</x:v>
+      </x:c>
+      <x:c r="M4" s="52" t="str">
         <x:v>Monthly</x:v>
       </x:c>
-      <x:c r="L4" s="31" t="n">
-        <x:v>10000</x:v>
-      </x:c>
-      <x:c r="M4" s="31" t="n">
-        <x:v/>
-      </x:c>
-      <x:c r="N4" s="31" t="str">
-        <x:v/>
-      </x:c>
-      <x:c r="O4" s="33" t="d">
-        <x:v>2019-10-11T00:00:00.0000000</x:v>
-      </x:c>
-      <x:c r="P4" s="33" t="d">
-        <x:v>2020-10-11T00:00:00.0000000</x:v>
-      </x:c>
-      <x:c r="Q4" s="31" t="str">
+      <x:c r="N4" s="52" t="n">
+        <x:v>61170</x:v>
+      </x:c>
+      <x:c r="O4" s="52" t="n">
+        <x:v>31</x:v>
+      </x:c>
+      <x:c r="P4" s="52" t="str">
+        <x:v>MPS</x:v>
+      </x:c>
+      <x:c r="Q4" s="54" t="d">
+        <x:v>2018-11-01T00:00:00.0000000</x:v>
+      </x:c>
+      <x:c r="R4" s="54" t="d">
+        <x:v>2020-08-31T00:00:00.0000000</x:v>
+      </x:c>
+      <x:c r="S4" s="52" t="str">
         <x:v>Active</x:v>
       </x:c>
-      <x:c r="R4" s="31" t="str">
+      <x:c r="T4" s="52" t="str">
         <x:v>No</x:v>
       </x:c>
-      <x:c r="S4" s="31" t="n">
+      <x:c r="U4" s="52" t="n">
         <x:v>39</x:v>
       </x:c>
-      <x:c r="T4" s="31" t="str">
+      <x:c r="V4" s="52" t="str">
         <x:v>DWS - CWB</x:v>
       </x:c>
     </x:row>
     <x:row r="5">
-      <x:c r="B5" s="31" t="str">
+      <x:c r="B5" s="52" t="str">
         <x:v>Data World Solutions Ltd</x:v>
       </x:c>
-      <x:c r="C5" s="31" t="str">
-        <x:v>S30171</x:v>
-      </x:c>
-      <x:c r="D5" s="31" t="str">
-        <x:v>Chan Ka Man</x:v>
-      </x:c>
-      <x:c r="E5" s="31" t="str">
+      <x:c r="C5" s="52" t="str">
+        <x:v>S31636</x:v>
+      </x:c>
+      <x:c r="D5" s="52" t="str">
+        <x:v>Chan Man Hung</x:v>
+      </x:c>
+      <x:c r="E5" s="52" t="str">
         <x:v>Unit A</x:v>
       </x:c>
-      <x:c r="F5" s="31" t="str">
-        <x:v>SOCIAL WORKER 社會工作員</x:v>
-      </x:c>
-      <x:c r="G5" s="33" t="d">
-        <x:v>2011-10-01T00:00:00.0000000</x:v>
-      </x:c>
-      <x:c r="H5" s="31" t="n">
-        <x:v>8.4754</x:v>
-      </x:c>
-      <x:c r="I5" s="31" t="str">
+      <x:c r="F5" s="52" t="str">
+        <x:v>General Staff 普通員工</x:v>
+      </x:c>
+      <x:c r="G5" s="52" t="str">
+        <x:v>CLERK</x:v>
+      </x:c>
+      <x:c r="H5" s="52" t="str">
+        <x:v>CLERK 文員</x:v>
+      </x:c>
+      <x:c r="I5" s="54" t="d">
+        <x:v>2017-03-01T00:00:00.0000000</x:v>
+      </x:c>
+      <x:c r="J5" s="52" t="n">
+        <x:v>3.0628</x:v>
+      </x:c>
+      <x:c r="K5" s="52" t="str">
         <x:v>AL10</x:v>
       </x:c>
-      <x:c r="J5" s="31" t="str">
-        <x:v>Statutory Holiday</x:v>
-      </x:c>
-      <x:c r="K5" s="31" t="str">
-        <x:v>Monthly</x:v>
-      </x:c>
-      <x:c r="L5" s="31" t="n">
-        <x:v>61170</x:v>
-      </x:c>
-      <x:c r="M5" s="31" t="n">
-        <x:v>31</x:v>
-      </x:c>
-      <x:c r="N5" s="31" t="str">
-        <x:v>MPS</x:v>
-      </x:c>
-      <x:c r="O5" s="33" t="d">
-        <x:v>2018-11-01T00:00:00.0000000</x:v>
-      </x:c>
-      <x:c r="P5" s="33" t="d">
-        <x:v>2020-08-31T00:00:00.0000000</x:v>
-      </x:c>
-      <x:c r="Q5" s="31" t="str">
+      <x:c r="L5" s="52" t="str">
+        <x:v>Bank Holiday</x:v>
+      </x:c>
+      <x:c r="M5" s="52" t="str">
+        <x:v>Hourly</x:v>
+      </x:c>
+      <x:c r="N5" s="52" t="n">
+        <x:v>70</x:v>
+      </x:c>
+      <x:c r="O5" s="52" t="n">
+        <x:v/>
+      </x:c>
+      <x:c r="P5" s="52" t="str">
+        <x:v/>
+      </x:c>
+      <x:c r="Q5" s="54" t="d">
+        <x:v>2018-09-01T00:00:00.0000000</x:v>
+      </x:c>
+      <x:c r="R5" s="54" t="d">
+        <x:v>2037-02-03T00:00:00.0000000</x:v>
+      </x:c>
+      <x:c r="S5" s="52" t="str">
         <x:v>Active</x:v>
       </x:c>
-      <x:c r="R5" s="31" t="str">
-        <x:v>No</x:v>
-      </x:c>
-      <x:c r="S5" s="31" t="n">
+      <x:c r="T5" s="52" t="str">
+        <x:v>Yes</x:v>
+      </x:c>
+      <x:c r="U5" s="52" t="n">
         <x:v>39</x:v>
       </x:c>
-      <x:c r="T5" s="31" t="str">
+      <x:c r="V5" s="52" t="str">
         <x:v>DWS - CWB</x:v>
       </x:c>
     </x:row>
     <x:row r="6">
-      <x:c r="B6" s="31" t="str">
+      <x:c r="B6" s="52" t="str">
         <x:v>Data World Solutions Ltd</x:v>
       </x:c>
-      <x:c r="C6" s="31" t="str">
-        <x:v>S31609</x:v>
-      </x:c>
-      <x:c r="D6" s="31" t="str">
-        <x:v>Chan Fai</x:v>
-      </x:c>
-      <x:c r="E6" s="31" t="str">
-        <x:v>Unit A</x:v>
-      </x:c>
-      <x:c r="F6" s="31" t="str">
-        <x:v>保健員</x:v>
-      </x:c>
-      <x:c r="G6" s="33" t="d">
-        <x:v>2016-01-01T00:00:00.0000000</x:v>
-      </x:c>
-      <x:c r="H6" s="31" t="n">
-        <x:v>4.2213</x:v>
-      </x:c>
-      <x:c r="I6" s="31" t="str">
-        <x:v>AL14</x:v>
-      </x:c>
-      <x:c r="J6" s="31" t="str">
-        <x:v>Bank Holiday</x:v>
-      </x:c>
-      <x:c r="K6" s="31" t="str">
+      <x:c r="C6" s="52" t="str">
+        <x:v>S31642</x:v>
+      </x:c>
+      <x:c r="D6" s="52" t="str">
+        <x:v>Chan Siu Fong</x:v>
+      </x:c>
+      <x:c r="E6" s="52" t="str">
+        <x:v>Unit C</x:v>
+      </x:c>
+      <x:c r="F6" s="52" t="str">
+        <x:v>General Staff 普通員工</x:v>
+      </x:c>
+      <x:c r="G6" s="52" t="str">
+        <x:v>CLERK</x:v>
+      </x:c>
+      <x:c r="H6" s="52" t="str">
+        <x:v>CLERK 文員</x:v>
+      </x:c>
+      <x:c r="I6" s="54" t="d">
+        <x:v>2018-01-02T00:00:00.0000000</x:v>
+      </x:c>
+      <x:c r="J6" s="52" t="n">
+        <x:v>2.2213</x:v>
+      </x:c>
+      <x:c r="K6" s="52" t="str">
+        <x:v>AL07</x:v>
+      </x:c>
+      <x:c r="L6" s="52" t="str">
+        <x:v>Statutory Holiday</x:v>
+      </x:c>
+      <x:c r="M6" s="52" t="str">
         <x:v>Monthly</x:v>
       </x:c>
-      <x:c r="L6" s="31" t="n">
-        <x:v>22005</x:v>
-      </x:c>
-      <x:c r="M6" s="31" t="n">
+      <x:c r="N6" s="52" t="n">
+        <x:v>9000</x:v>
+      </x:c>
+      <x:c r="O6" s="52" t="n">
         <x:v/>
       </x:c>
-      <x:c r="N6" s="31" t="str">
+      <x:c r="P6" s="52" t="str">
         <x:v/>
       </x:c>
-      <x:c r="O6" s="33" t="d">
-        <x:v>2019-08-14T00:00:00.0000000</x:v>
-      </x:c>
-      <x:c r="P6" s="33" t="d">
-        <x:v>2034-05-05T00:00:00.0000000</x:v>
-      </x:c>
-      <x:c r="Q6" s="31" t="str">
+      <x:c r="Q6" s="54" t="d">
+        <x:v>2019-08-01T00:00:00.0000000</x:v>
+      </x:c>
+      <x:c r="R6" s="54" t="d">
+        <x:v>2040-02-01T00:00:00.0000000</x:v>
+      </x:c>
+      <x:c r="S6" s="52" t="str">
         <x:v>Active</x:v>
       </x:c>
-      <x:c r="R6" s="31" t="str">
+      <x:c r="T6" s="52" t="str">
         <x:v>No</x:v>
       </x:c>
-      <x:c r="S6" s="31" t="n">
-        <x:v>39</x:v>
-      </x:c>
-      <x:c r="T6" s="31" t="str">
-        <x:v>DWS - CWB</x:v>
+      <x:c r="U6" s="52" t="n">
+        <x:v>40</x:v>
+      </x:c>
+      <x:c r="V6" s="52" t="str">
+        <x:v>TST</x:v>
       </x:c>
     </x:row>
     <x:row r="7">
-      <x:c r="B7" s="31" t="str">
+      <x:c r="B7" s="52" t="str">
         <x:v>Data World Solutions Ltd</x:v>
       </x:c>
-      <x:c r="C7" s="31" t="str">
-        <x:v>S31610</x:v>
-      </x:c>
-      <x:c r="D7" s="31" t="str">
-        <x:v>Chan Shun</x:v>
-      </x:c>
-      <x:c r="E7" s="31" t="str">
+      <x:c r="C7" s="52" t="str">
+        <x:v>AA100818</x:v>
+      </x:c>
+      <x:c r="D7" s="52" t="str">
+        <x:v>Chan Tai man 10</x:v>
+      </x:c>
+      <x:c r="E7" s="52" t="str">
         <x:v>Unit A</x:v>
       </x:c>
-      <x:c r="F7" s="31" t="str">
-        <x:v>保健員</x:v>
-      </x:c>
-      <x:c r="G7" s="33" t="d">
-        <x:v>2016-01-01T00:00:00.0000000</x:v>
-      </x:c>
-      <x:c r="H7" s="31" t="n">
-        <x:v>4.2213</x:v>
-      </x:c>
-      <x:c r="I7" s="31" t="str">
-        <x:v>AL14</x:v>
-      </x:c>
-      <x:c r="J7" s="31" t="str">
+      <x:c r="F7" s="52" t="str">
+        <x:v>General Staff 普通員工</x:v>
+      </x:c>
+      <x:c r="G7" s="52" t="str">
+        <x:v>CWIII</x:v>
+      </x:c>
+      <x:c r="H7" s="52" t="str">
+        <x:v>CARE WORKER 護理員</x:v>
+      </x:c>
+      <x:c r="I7" s="54" t="d">
+        <x:v>2019-10-11T00:00:00.0000000</x:v>
+      </x:c>
+      <x:c r="J7" s="52" t="n">
+        <x:v>0.4508</x:v>
+      </x:c>
+      <x:c r="K7" s="52" t="str">
+        <x:v>AL07</x:v>
+      </x:c>
+      <x:c r="L7" s="52" t="str">
         <x:v>Bank Holiday</x:v>
       </x:c>
-      <x:c r="K7" s="31" t="str">
+      <x:c r="M7" s="52" t="str">
         <x:v>Monthly</x:v>
       </x:c>
-      <x:c r="L7" s="31" t="n">
+      <x:c r="N7" s="52" t="n">
         <x:v>10000</x:v>
       </x:c>
-      <x:c r="M7" s="31" t="n">
+      <x:c r="O7" s="52" t="n">
         <x:v/>
       </x:c>
-      <x:c r="N7" s="31" t="str">
+      <x:c r="P7" s="52" t="str">
         <x:v/>
       </x:c>
-      <x:c r="O7" s="33" t="d">
-        <x:v>2018-12-01T00:00:00.0000000</x:v>
-      </x:c>
-      <x:c r="P7" s="33" t="d">
-        <x:v>2046-06-06T00:00:00.0000000</x:v>
-      </x:c>
-      <x:c r="Q7" s="31" t="str">
+      <x:c r="Q7" s="54" t="d">
+        <x:v>2019-10-11T00:00:00.0000000</x:v>
+      </x:c>
+      <x:c r="R7" s="54" t="d">
+        <x:v>2020-10-11T00:00:00.0000000</x:v>
+      </x:c>
+      <x:c r="S7" s="52" t="str">
         <x:v>Active</x:v>
       </x:c>
-      <x:c r="R7" s="31" t="str">
+      <x:c r="T7" s="52" t="str">
         <x:v>No</x:v>
       </x:c>
-      <x:c r="S7" s="31" t="n">
+      <x:c r="U7" s="52" t="n">
         <x:v>39</x:v>
       </x:c>
-      <x:c r="T7" s="31" t="str">
+      <x:c r="V7" s="52" t="str">
         <x:v>DWS - CWB</x:v>
       </x:c>
     </x:row>
     <x:row r="8">
-      <x:c r="B8" s="31" t="str">
+      <x:c r="B8" s="52" t="str">
         <x:v>Data World Solutions Ltd</x:v>
       </x:c>
-      <x:c r="C8" s="31" t="str">
-        <x:v>S31611</x:v>
-      </x:c>
-      <x:c r="D8" s="31" t="str">
-        <x:v>Chan Hang</x:v>
-      </x:c>
-      <x:c r="E8" s="31" t="str">
+      <x:c r="C8" s="52" t="str">
+        <x:v>S31609</x:v>
+      </x:c>
+      <x:c r="D8" s="52" t="str">
+        <x:v>Chan Fai</x:v>
+      </x:c>
+      <x:c r="E8" s="52" t="str">
         <x:v>Unit A</x:v>
       </x:c>
-      <x:c r="F8" s="31" t="str">
-        <x:v>主任</x:v>
-      </x:c>
-      <x:c r="G8" s="33" t="d">
+      <x:c r="F8" s="52" t="str">
+        <x:v>General Staff 普通員工</x:v>
+      </x:c>
+      <x:c r="G8" s="52" t="str">
+        <x:v>HEALTH WORKERS</x:v>
+      </x:c>
+      <x:c r="H8" s="52" t="str">
+        <x:v>保健員</x:v>
+      </x:c>
+      <x:c r="I8" s="54" t="d">
         <x:v>2016-01-01T00:00:00.0000000</x:v>
       </x:c>
-      <x:c r="H8" s="31" t="n">
-        <x:v>4.2213</x:v>
-      </x:c>
-      <x:c r="I8" s="31" t="str">
+      <x:c r="J8" s="52" t="n">
+        <x:v>4.224</x:v>
+      </x:c>
+      <x:c r="K8" s="52" t="str">
         <x:v>AL14</x:v>
       </x:c>
-      <x:c r="J8" s="31" t="str">
+      <x:c r="L8" s="52" t="str">
         <x:v>Bank Holiday</x:v>
       </x:c>
-      <x:c r="K8" s="31" t="str">
+      <x:c r="M8" s="52" t="str">
         <x:v>Monthly</x:v>
       </x:c>
-      <x:c r="L8" s="31" t="n">
-        <x:v>30020</x:v>
-      </x:c>
-      <x:c r="M8" s="31" t="n">
-        <x:v>17</x:v>
-      </x:c>
-      <x:c r="N8" s="31" t="str">
-        <x:v>MPS</x:v>
-      </x:c>
-      <x:c r="O8" s="33" t="d">
-        <x:v>2016-04-01T00:00:00.0000000</x:v>
-      </x:c>
-      <x:c r="P8" s="33" t="d">
-        <x:v>2048-01-01T00:00:00.0000000</x:v>
-      </x:c>
-      <x:c r="Q8" s="31" t="str">
+      <x:c r="N8" s="52" t="n">
+        <x:v>22005</x:v>
+      </x:c>
+      <x:c r="O8" s="52" t="n">
+        <x:v/>
+      </x:c>
+      <x:c r="P8" s="52" t="str">
+        <x:v/>
+      </x:c>
+      <x:c r="Q8" s="54" t="d">
+        <x:v>2019-08-14T00:00:00.0000000</x:v>
+      </x:c>
+      <x:c r="R8" s="54" t="d">
+        <x:v>2034-05-05T00:00:00.0000000</x:v>
+      </x:c>
+      <x:c r="S8" s="52" t="str">
         <x:v>Active</x:v>
       </x:c>
-      <x:c r="R8" s="31" t="str">
+      <x:c r="T8" s="52" t="str">
         <x:v>No</x:v>
       </x:c>
-      <x:c r="S8" s="31" t="n">
+      <x:c r="U8" s="52" t="n">
         <x:v>39</x:v>
       </x:c>
-      <x:c r="T8" s="31" t="str">
+      <x:c r="V8" s="52" t="str">
         <x:v>DWS - CWB</x:v>
       </x:c>
     </x:row>
     <x:row r="9">
-      <x:c r="B9" s="31" t="str">
+      <x:c r="B9" s="52" t="str">
         <x:v>Data World Solutions Ltd</x:v>
       </x:c>
-      <x:c r="C9" s="31" t="str">
-        <x:v>S31612</x:v>
-      </x:c>
-      <x:c r="D9" s="31" t="str">
-        <x:v>Chan Ka</x:v>
-      </x:c>
-      <x:c r="E9" s="31" t="str">
+      <x:c r="C9" s="52" t="str">
+        <x:v>S31610</x:v>
+      </x:c>
+      <x:c r="D9" s="52" t="str">
+        <x:v>Chan Shun</x:v>
+      </x:c>
+      <x:c r="E9" s="52" t="str">
         <x:v>Unit A</x:v>
       </x:c>
-      <x:c r="F9" s="31" t="str">
-        <x:v>OFFICER 主任</x:v>
-      </x:c>
-      <x:c r="G9" s="33" t="d">
+      <x:c r="F9" s="52" t="str">
+        <x:v>General Staff 普通員工</x:v>
+      </x:c>
+      <x:c r="G9" s="52" t="str">
+        <x:v>HEALTH WORKERS</x:v>
+      </x:c>
+      <x:c r="H9" s="52" t="str">
+        <x:v>保健員</x:v>
+      </x:c>
+      <x:c r="I9" s="54" t="d">
         <x:v>2016-01-01T00:00:00.0000000</x:v>
       </x:c>
-      <x:c r="H9" s="31" t="n">
-        <x:v>4.2213</x:v>
-      </x:c>
-      <x:c r="I9" s="31" t="str">
+      <x:c r="J9" s="52" t="n">
+        <x:v>4.224</x:v>
+      </x:c>
+      <x:c r="K9" s="52" t="str">
         <x:v>AL14</x:v>
       </x:c>
-      <x:c r="J9" s="31" t="str">
+      <x:c r="L9" s="52" t="str">
         <x:v>Bank Holiday</x:v>
       </x:c>
-      <x:c r="K9" s="31" t="str">
+      <x:c r="M9" s="52" t="str">
         <x:v>Monthly</x:v>
       </x:c>
-      <x:c r="L9" s="31" t="n">
-        <x:v>39554</x:v>
-      </x:c>
-      <x:c r="M9" s="31" t="n">
+      <x:c r="N9" s="52" t="n">
+        <x:v>10000</x:v>
+      </x:c>
+      <x:c r="O9" s="52" t="n">
         <x:v/>
       </x:c>
-      <x:c r="N9" s="31" t="str">
+      <x:c r="P9" s="52" t="str">
         <x:v/>
       </x:c>
-      <x:c r="O9" s="33" t="d">
-        <x:v>2016-04-01T00:00:00.0000000</x:v>
-      </x:c>
-      <x:c r="P9" s="33" t="d">
-        <x:v>2048-01-01T00:00:00.0000000</x:v>
-      </x:c>
-      <x:c r="Q9" s="31" t="str">
+      <x:c r="Q9" s="54" t="d">
+        <x:v>2018-12-01T00:00:00.0000000</x:v>
+      </x:c>
+      <x:c r="R9" s="54" t="d">
+        <x:v>2046-06-06T00:00:00.0000000</x:v>
+      </x:c>
+      <x:c r="S9" s="52" t="str">
         <x:v>Active</x:v>
       </x:c>
-      <x:c r="R9" s="31" t="str">
+      <x:c r="T9" s="52" t="str">
         <x:v>No</x:v>
       </x:c>
-      <x:c r="S9" s="31" t="n">
+      <x:c r="U9" s="52" t="n">
         <x:v>39</x:v>
       </x:c>
-      <x:c r="T9" s="31" t="str">
+      <x:c r="V9" s="52" t="str">
         <x:v>DWS - CWB</x:v>
       </x:c>
     </x:row>
     <x:row r="10">
-      <x:c r="B10" s="31" t="str">
+      <x:c r="B10" s="52" t="str">
         <x:v>Data World Solutions Ltd</x:v>
       </x:c>
-      <x:c r="C10" s="31" t="str">
-        <x:v>S31636</x:v>
-      </x:c>
-      <x:c r="D10" s="31" t="str">
-        <x:v>Chan Man Hung</x:v>
-      </x:c>
-      <x:c r="E10" s="31" t="str">
+      <x:c r="C10" s="52" t="str">
+        <x:v>S31643</x:v>
+      </x:c>
+      <x:c r="D10" s="52" t="str">
+        <x:v>Chan Li Chun</x:v>
+      </x:c>
+      <x:c r="E10" s="52" t="str">
         <x:v>Unit A</x:v>
       </x:c>
-      <x:c r="F10" s="31" t="str">
-        <x:v>CLERK 文員</x:v>
-      </x:c>
-      <x:c r="G10" s="33" t="d">
-        <x:v>2017-03-01T00:00:00.0000000</x:v>
-      </x:c>
-      <x:c r="H10" s="31" t="n">
-        <x:v>3.0601</x:v>
-      </x:c>
-      <x:c r="I10" s="31" t="str">
-        <x:v>AL10</x:v>
-      </x:c>
-      <x:c r="J10" s="31" t="str">
-        <x:v>Bank Holiday</x:v>
-      </x:c>
-      <x:c r="K10" s="31" t="str">
+      <x:c r="F10" s="52" t="str">
+        <x:v>General Staff 普通員工</x:v>
+      </x:c>
+      <x:c r="G10" s="52" t="str">
+        <x:v>HEALTH WORKERS</x:v>
+      </x:c>
+      <x:c r="H10" s="52" t="str">
+        <x:v>保健員</x:v>
+      </x:c>
+      <x:c r="I10" s="54" t="d">
+        <x:v>2018-01-02T00:00:00.0000000</x:v>
+      </x:c>
+      <x:c r="J10" s="52" t="n">
+        <x:v>2.2213</x:v>
+      </x:c>
+      <x:c r="K10" s="52" t="str">
+        <x:v>AL0</x:v>
+      </x:c>
+      <x:c r="L10" s="52" t="str">
+        <x:v>Statutory Holiday</x:v>
+      </x:c>
+      <x:c r="M10" s="52" t="str">
         <x:v>Hourly</x:v>
       </x:c>
-      <x:c r="L10" s="31" t="n">
-        <x:v>70</x:v>
-      </x:c>
-      <x:c r="M10" s="31" t="n">
+      <x:c r="N10" s="52" t="n">
+        <x:v>50</x:v>
+      </x:c>
+      <x:c r="O10" s="52" t="n">
         <x:v/>
       </x:c>
-      <x:c r="N10" s="31" t="str">
+      <x:c r="P10" s="52" t="str">
         <x:v/>
       </x:c>
-      <x:c r="O10" s="33" t="d">
-        <x:v>2018-09-01T00:00:00.0000000</x:v>
-      </x:c>
-      <x:c r="P10" s="33" t="d">
-        <x:v>2037-02-03T00:00:00.0000000</x:v>
-      </x:c>
-      <x:c r="Q10" s="31" t="str">
+      <x:c r="Q10" s="54" t="d">
+        <x:v>2018-01-02T00:00:00.0000000</x:v>
+      </x:c>
+      <x:c r="R10" s="54" t="d">
+        <x:v>2045-01-01T00:00:00.0000000</x:v>
+      </x:c>
+      <x:c r="S10" s="52" t="str">
         <x:v>Active</x:v>
       </x:c>
-      <x:c r="R10" s="31" t="str">
+      <x:c r="T10" s="52" t="str">
         <x:v>Yes</x:v>
       </x:c>
-      <x:c r="S10" s="31" t="n">
+      <x:c r="U10" s="52" t="n">
         <x:v>39</x:v>
       </x:c>
-      <x:c r="T10" s="31" t="str">
+      <x:c r="V10" s="52" t="str">
         <x:v>DWS - CWB</x:v>
       </x:c>
     </x:row>
     <x:row r="11">
-      <x:c r="B11" s="31" t="str">
+      <x:c r="B11" s="52" t="str">
         <x:v>Data World Solutions Ltd</x:v>
       </x:c>
-      <x:c r="C11" s="31" t="str">
-        <x:v>S31642</x:v>
-      </x:c>
-      <x:c r="D11" s="31" t="str">
-        <x:v>Chan Siu Fong</x:v>
-      </x:c>
-      <x:c r="E11" s="31" t="str">
-        <x:v>Unit C</x:v>
-      </x:c>
-      <x:c r="F11" s="31" t="str">
-        <x:v>CLERK 文員</x:v>
-      </x:c>
-      <x:c r="G11" s="33" t="d">
+      <x:c r="C11" s="52" t="str">
+        <x:v>S31644</x:v>
+      </x:c>
+      <x:c r="D11" s="52" t="str">
+        <x:v>Cheung Li Chun</x:v>
+      </x:c>
+      <x:c r="E11" s="52" t="str">
+        <x:v>Unit A</x:v>
+      </x:c>
+      <x:c r="F11" s="52" t="str">
+        <x:v>General Staff 普通員工</x:v>
+      </x:c>
+      <x:c r="G11" s="52" t="str">
+        <x:v>HEALTH WORKERS</x:v>
+      </x:c>
+      <x:c r="H11" s="52" t="str">
+        <x:v>保健員</x:v>
+      </x:c>
+      <x:c r="I11" s="54" t="d">
         <x:v>2018-01-02T00:00:00.0000000</x:v>
       </x:c>
-      <x:c r="H11" s="31" t="n">
-        <x:v>2.2186</x:v>
-      </x:c>
-      <x:c r="I11" s="31" t="str">
-        <x:v>AL07</x:v>
-      </x:c>
-      <x:c r="J11" s="31" t="str">
+      <x:c r="J11" s="52" t="n">
+        <x:v>2.2213</x:v>
+      </x:c>
+      <x:c r="K11" s="52" t="str">
+        <x:v>AL0</x:v>
+      </x:c>
+      <x:c r="L11" s="52" t="str">
         <x:v>Statutory Holiday</x:v>
       </x:c>
-      <x:c r="K11" s="31" t="str">
-        <x:v>Monthly</x:v>
-      </x:c>
-      <x:c r="L11" s="31" t="n">
-        <x:v>9000</x:v>
-      </x:c>
-      <x:c r="M11" s="31" t="n">
+      <x:c r="M11" s="52" t="str">
+        <x:v>Hourly</x:v>
+      </x:c>
+      <x:c r="N11" s="52" t="n">
+        <x:v>50</x:v>
+      </x:c>
+      <x:c r="O11" s="52" t="n">
         <x:v/>
       </x:c>
-      <x:c r="N11" s="31" t="str">
+      <x:c r="P11" s="52" t="str">
         <x:v/>
       </x:c>
-      <x:c r="O11" s="33" t="d">
-        <x:v>2019-08-01T00:00:00.0000000</x:v>
-      </x:c>
-      <x:c r="P11" s="33" t="d">
-        <x:v>2040-02-01T00:00:00.0000000</x:v>
-      </x:c>
-      <x:c r="Q11" s="31" t="str">
+      <x:c r="Q11" s="54" t="d">
+        <x:v>2018-01-02T00:00:00.0000000</x:v>
+      </x:c>
+      <x:c r="R11" s="54" t="d">
+        <x:v>2041-03-01T00:00:00.0000000</x:v>
+      </x:c>
+      <x:c r="S11" s="52" t="str">
         <x:v>Active</x:v>
       </x:c>
-      <x:c r="R11" s="31" t="str">
-        <x:v>No</x:v>
-      </x:c>
-      <x:c r="S11" s="31" t="n">
-        <x:v>40</x:v>
-      </x:c>
-      <x:c r="T11" s="31" t="str">
-        <x:v>TST</x:v>
+      <x:c r="T11" s="52" t="str">
+        <x:v>Yes</x:v>
+      </x:c>
+      <x:c r="U11" s="52" t="n">
+        <x:v>39</x:v>
+      </x:c>
+      <x:c r="V11" s="52" t="str">
+        <x:v>DWS - CWB</x:v>
       </x:c>
     </x:row>
     <x:row r="12">
-      <x:c r="B12" s="31" t="str">
+      <x:c r="B12" s="52" t="str">
         <x:v>Data World Solutions Ltd</x:v>
       </x:c>
-      <x:c r="C12" s="31" t="str">
-        <x:v>S31643</x:v>
-      </x:c>
-      <x:c r="D12" s="31" t="str">
-        <x:v>Chan Li Chun</x:v>
-      </x:c>
-      <x:c r="E12" s="31" t="str">
+      <x:c r="C12" s="52" t="str">
+        <x:v>S31645</x:v>
+      </x:c>
+      <x:c r="D12" s="52" t="str">
+        <x:v>Chan Siu Li</x:v>
+      </x:c>
+      <x:c r="E12" s="52" t="str">
         <x:v>Unit A</x:v>
       </x:c>
-      <x:c r="F12" s="31" t="str">
+      <x:c r="F12" s="52" t="str">
+        <x:v>General Staff 普通員工</x:v>
+      </x:c>
+      <x:c r="G12" s="52" t="str">
+        <x:v>HEALTH WORKERS</x:v>
+      </x:c>
+      <x:c r="H12" s="52" t="str">
         <x:v>保健員</x:v>
       </x:c>
-      <x:c r="G12" s="33" t="d">
+      <x:c r="I12" s="54" t="d">
         <x:v>2018-01-02T00:00:00.0000000</x:v>
       </x:c>
-      <x:c r="H12" s="31" t="n">
-        <x:v>2.2186</x:v>
-      </x:c>
-      <x:c r="I12" s="31" t="str">
+      <x:c r="J12" s="52" t="n">
+        <x:v>2.2213</x:v>
+      </x:c>
+      <x:c r="K12" s="52" t="str">
         <x:v>AL0</x:v>
       </x:c>
-      <x:c r="J12" s="31" t="str">
+      <x:c r="L12" s="52" t="str">
         <x:v>Statutory Holiday</x:v>
       </x:c>
-      <x:c r="K12" s="31" t="str">
+      <x:c r="M12" s="52" t="str">
         <x:v>Hourly</x:v>
       </x:c>
-      <x:c r="L12" s="31" t="n">
+      <x:c r="N12" s="52" t="n">
         <x:v>50</x:v>
       </x:c>
-      <x:c r="M12" s="31" t="n">
+      <x:c r="O12" s="52" t="n">
         <x:v/>
       </x:c>
-      <x:c r="N12" s="31" t="str">
+      <x:c r="P12" s="52" t="str">
         <x:v/>
       </x:c>
-      <x:c r="O12" s="33" t="d">
+      <x:c r="Q12" s="54" t="d">
         <x:v>2018-01-02T00:00:00.0000000</x:v>
       </x:c>
-      <x:c r="P12" s="33" t="d">
-        <x:v>2045-01-01T00:00:00.0000000</x:v>
-      </x:c>
-      <x:c r="Q12" s="31" t="str">
+      <x:c r="R12" s="54" t="d">
+        <x:v>2050-12-15T00:00:00.0000000</x:v>
+      </x:c>
+      <x:c r="S12" s="52" t="str">
         <x:v>Active</x:v>
       </x:c>
-      <x:c r="R12" s="31" t="str">
+      <x:c r="T12" s="52" t="str">
         <x:v>Yes</x:v>
       </x:c>
-      <x:c r="S12" s="31" t="n">
+      <x:c r="U12" s="52" t="n">
         <x:v>39</x:v>
       </x:c>
-      <x:c r="T12" s="31" t="str">
+      <x:c r="V12" s="52" t="str">
         <x:v>DWS - CWB</x:v>
       </x:c>
     </x:row>
     <x:row r="13">
-      <x:c r="B13" s="31" t="str">
+      <x:c r="B13" s="52" t="str">
         <x:v>Data World Solutions Ltd</x:v>
       </x:c>
-      <x:c r="C13" s="31" t="str">
-        <x:v>S31644</x:v>
-      </x:c>
-      <x:c r="D13" s="31" t="str">
-        <x:v>Cheung Li Chun</x:v>
-      </x:c>
-      <x:c r="E13" s="31" t="str">
-        <x:v>Unit A</x:v>
-      </x:c>
-      <x:c r="F13" s="31" t="str">
+      <x:c r="C13" s="52" t="str">
+        <x:v>S31647</x:v>
+      </x:c>
+      <x:c r="D13" s="52" t="str">
+        <x:v>Chan guan guan</x:v>
+      </x:c>
+      <x:c r="E13" s="52" t="str">
+        <x:v>Unit B</x:v>
+      </x:c>
+      <x:c r="F13" s="52" t="str">
+        <x:v>General Staff 普通員工</x:v>
+      </x:c>
+      <x:c r="G13" s="52" t="str">
+        <x:v>HEALTH WORKERS</x:v>
+      </x:c>
+      <x:c r="H13" s="52" t="str">
         <x:v>保健員</x:v>
       </x:c>
-      <x:c r="G13" s="33" t="d">
-        <x:v>2018-01-02T00:00:00.0000000</x:v>
-      </x:c>
-      <x:c r="H13" s="31" t="n">
-        <x:v>2.2186</x:v>
-      </x:c>
-      <x:c r="I13" s="31" t="str">
-        <x:v>AL0</x:v>
-      </x:c>
-      <x:c r="J13" s="31" t="str">
+      <x:c r="I13" s="54" t="d">
+        <x:v>2015-11-15T00:00:00.0000000</x:v>
+      </x:c>
+      <x:c r="J13" s="52" t="n">
+        <x:v>4.3552</x:v>
+      </x:c>
+      <x:c r="K13" s="52" t="str">
+        <x:v>AL07</x:v>
+      </x:c>
+      <x:c r="L13" s="52" t="str">
         <x:v>Statutory Holiday</x:v>
       </x:c>
-      <x:c r="K13" s="31" t="str">
-        <x:v>Hourly</x:v>
-      </x:c>
-      <x:c r="L13" s="31" t="n">
-        <x:v>50</x:v>
-      </x:c>
-      <x:c r="M13" s="31" t="n">
+      <x:c r="M13" s="52" t="str">
+        <x:v>Monthly</x:v>
+      </x:c>
+      <x:c r="N13" s="52" t="n">
+        <x:v>15000</x:v>
+      </x:c>
+      <x:c r="O13" s="52" t="n">
         <x:v/>
       </x:c>
-      <x:c r="N13" s="31" t="str">
+      <x:c r="P13" s="52" t="str">
         <x:v/>
       </x:c>
-      <x:c r="O13" s="33" t="d">
-        <x:v>2018-01-02T00:00:00.0000000</x:v>
-      </x:c>
-      <x:c r="P13" s="33" t="d">
-        <x:v>2041-03-01T00:00:00.0000000</x:v>
-      </x:c>
-      <x:c r="Q13" s="31" t="str">
+      <x:c r="Q13" s="54" t="d">
+        <x:v>2019-09-10T00:00:00.0000000</x:v>
+      </x:c>
+      <x:c r="R13" s="54" t="d">
+        <x:v>2045-01-01T00:00:00.0000000</x:v>
+      </x:c>
+      <x:c r="S13" s="52" t="str">
         <x:v>Active</x:v>
       </x:c>
-      <x:c r="R13" s="31" t="str">
-        <x:v>Yes</x:v>
-      </x:c>
-      <x:c r="S13" s="31" t="n">
-        <x:v>39</x:v>
-      </x:c>
-      <x:c r="T13" s="31" t="str">
-        <x:v>DWS - CWB</x:v>
+      <x:c r="T13" s="52" t="str">
+        <x:v>No</x:v>
+      </x:c>
+      <x:c r="U13" s="52" t="n">
+        <x:v>24</x:v>
+      </x:c>
+      <x:c r="V13" s="52" t="str">
+        <x:v>CARE</x:v>
       </x:c>
     </x:row>
     <x:row r="14">
-      <x:c r="B14" s="31" t="str">
+      <x:c r="B14" s="52" t="str">
         <x:v>Data World Solutions Ltd</x:v>
       </x:c>
-      <x:c r="C14" s="31" t="str">
-        <x:v>S31645</x:v>
-      </x:c>
-      <x:c r="D14" s="31" t="str">
-        <x:v>Chan Siu Li</x:v>
-      </x:c>
-      <x:c r="E14" s="31" t="str">
+      <x:c r="C14" s="52" t="str">
+        <x:v>S31662</x:v>
+      </x:c>
+      <x:c r="D14" s="52" t="str">
+        <x:v>Chan Kit</x:v>
+      </x:c>
+      <x:c r="E14" s="52" t="str">
         <x:v>Unit A</x:v>
       </x:c>
-      <x:c r="F14" s="31" t="str">
+      <x:c r="F14" s="52" t="str">
+        <x:v>General Staff 普通員工</x:v>
+      </x:c>
+      <x:c r="G14" s="52" t="str">
+        <x:v>HEALTH WORKERS</x:v>
+      </x:c>
+      <x:c r="H14" s="52" t="str">
         <x:v>保健員</x:v>
       </x:c>
-      <x:c r="G14" s="33" t="d">
-        <x:v>2018-01-02T00:00:00.0000000</x:v>
-      </x:c>
-      <x:c r="H14" s="31" t="n">
-        <x:v>2.2186</x:v>
-      </x:c>
-      <x:c r="I14" s="31" t="str">
-        <x:v>AL0</x:v>
-      </x:c>
-      <x:c r="J14" s="31" t="str">
-        <x:v>Statutory Holiday</x:v>
-      </x:c>
-      <x:c r="K14" s="31" t="str">
-        <x:v>Hourly</x:v>
-      </x:c>
-      <x:c r="L14" s="31" t="n">
-        <x:v>50</x:v>
-      </x:c>
-      <x:c r="M14" s="31" t="n">
+      <x:c r="I14" s="54" t="d">
+        <x:v>2019-01-01T00:00:00.0000000</x:v>
+      </x:c>
+      <x:c r="J14" s="52" t="n">
+        <x:v>1.224</x:v>
+      </x:c>
+      <x:c r="K14" s="52" t="str">
+        <x:v>AL14</x:v>
+      </x:c>
+      <x:c r="L14" s="52" t="str">
+        <x:v>Bank Holiday</x:v>
+      </x:c>
+      <x:c r="M14" s="52" t="str">
+        <x:v>Monthly</x:v>
+      </x:c>
+      <x:c r="N14" s="52" t="n">
+        <x:v>15000</x:v>
+      </x:c>
+      <x:c r="O14" s="52" t="n">
+        <x:v>4</x:v>
+      </x:c>
+      <x:c r="P14" s="52" t="str">
         <x:v/>
       </x:c>
-      <x:c r="N14" s="31" t="str">
-        <x:v/>
-      </x:c>
-      <x:c r="O14" s="33" t="d">
-        <x:v>2018-01-02T00:00:00.0000000</x:v>
-      </x:c>
-      <x:c r="P14" s="33" t="d">
-        <x:v>2050-12-15T00:00:00.0000000</x:v>
-      </x:c>
-      <x:c r="Q14" s="31" t="str">
+      <x:c r="Q14" s="54" t="d">
+        <x:v>2019-01-01T00:00:00.0000000</x:v>
+      </x:c>
+      <x:c r="R14" s="54" t="d">
+        <x:v>2045-01-01T00:00:00.0000000</x:v>
+      </x:c>
+      <x:c r="S14" s="52" t="str">
         <x:v>Active</x:v>
       </x:c>
-      <x:c r="R14" s="31" t="str">
-        <x:v>Yes</x:v>
-      </x:c>
-      <x:c r="S14" s="31" t="n">
+      <x:c r="T14" s="52" t="str">
+        <x:v>No</x:v>
+      </x:c>
+      <x:c r="U14" s="52" t="n">
         <x:v>39</x:v>
       </x:c>
-      <x:c r="T14" s="31" t="str">
+      <x:c r="V14" s="52" t="str">
         <x:v>DWS - CWB</x:v>
       </x:c>
     </x:row>
     <x:row r="15">
-      <x:c r="B15" s="31" t="str">
+      <x:c r="B15" s="52" t="str">
         <x:v>Data World Solutions Ltd</x:v>
       </x:c>
-      <x:c r="C15" s="31" t="str">
-        <x:v>S31647</x:v>
-      </x:c>
-      <x:c r="D15" s="31" t="str">
-        <x:v>Chan guan guan</x:v>
-      </x:c>
-      <x:c r="E15" s="31" t="str">
-        <x:v>Unit B</x:v>
-      </x:c>
-      <x:c r="F15" s="31" t="str">
-        <x:v>保健員</x:v>
-      </x:c>
-      <x:c r="G15" s="33" t="d">
-        <x:v>2015-11-15T00:00:00.0000000</x:v>
-      </x:c>
-      <x:c r="H15" s="31" t="n">
-        <x:v>4.3525</x:v>
-      </x:c>
-      <x:c r="I15" s="31" t="str">
-        <x:v>AL07</x:v>
-      </x:c>
-      <x:c r="J15" s="31" t="str">
-        <x:v>Statutory Holiday</x:v>
-      </x:c>
-      <x:c r="K15" s="31" t="str">
+      <x:c r="C15" s="52" t="str">
+        <x:v>S31649</x:v>
+      </x:c>
+      <x:c r="D15" s="52" t="str">
+        <x:v>Chan Chi Man</x:v>
+      </x:c>
+      <x:c r="E15" s="52" t="str">
+        <x:v>Unit A</x:v>
+      </x:c>
+      <x:c r="F15" s="52" t="str">
+        <x:v>General Staff 普通員工</x:v>
+      </x:c>
+      <x:c r="G15" s="52" t="str">
+        <x:v>HW2</x:v>
+      </x:c>
+      <x:c r="H15" s="52" t="str">
+        <x:v>福利服務助理</x:v>
+      </x:c>
+      <x:c r="I15" s="54" t="d">
+        <x:v>2018-03-08T00:00:00.0000000</x:v>
+      </x:c>
+      <x:c r="J15" s="52" t="n">
+        <x:v>2.0437</x:v>
+      </x:c>
+      <x:c r="K15" s="52" t="str">
+        <x:v>AL14</x:v>
+      </x:c>
+      <x:c r="L15" s="52" t="str">
+        <x:v>Bank Holiday</x:v>
+      </x:c>
+      <x:c r="M15" s="52" t="str">
         <x:v>Monthly</x:v>
       </x:c>
-      <x:c r="L15" s="31" t="n">
-        <x:v>15000</x:v>
-      </x:c>
-      <x:c r="M15" s="31" t="n">
-        <x:v/>
-      </x:c>
-      <x:c r="N15" s="31" t="str">
-        <x:v/>
-      </x:c>
-      <x:c r="O15" s="33" t="d">
-        <x:v>2019-09-10T00:00:00.0000000</x:v>
-      </x:c>
-      <x:c r="P15" s="33" t="d">
+      <x:c r="N15" s="52" t="n">
+        <x:v>20650</x:v>
+      </x:c>
+      <x:c r="O15" s="52" t="n">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="P15" s="52" t="str">
+        <x:v>MPS</x:v>
+      </x:c>
+      <x:c r="Q15" s="54" t="d">
+        <x:v>2018-03-08T00:00:00.0000000</x:v>
+      </x:c>
+      <x:c r="R15" s="54" t="d">
         <x:v>2045-01-01T00:00:00.0000000</x:v>
       </x:c>
-      <x:c r="Q15" s="31" t="str">
+      <x:c r="S15" s="52" t="str">
         <x:v>Active</x:v>
       </x:c>
-      <x:c r="R15" s="31" t="str">
+      <x:c r="T15" s="52" t="str">
         <x:v>No</x:v>
       </x:c>
-      <x:c r="S15" s="31" t="n">
-        <x:v>24</x:v>
-      </x:c>
-      <x:c r="T15" s="31" t="str">
-        <x:v>CARE</x:v>
+      <x:c r="U15" s="52" t="n">
+        <x:v>39</x:v>
+      </x:c>
+      <x:c r="V15" s="52" t="str">
+        <x:v>DWS - CWB</x:v>
       </x:c>
     </x:row>
     <x:row r="16">
-      <x:c r="B16" s="31" t="str">
+      <x:c r="B16" s="52" t="str">
         <x:v>Data World Solutions Ltd</x:v>
       </x:c>
-      <x:c r="C16" s="31" t="str">
-        <x:v>S31649</x:v>
-      </x:c>
-      <x:c r="D16" s="31" t="str">
-        <x:v>Chan Chi Man</x:v>
-      </x:c>
-      <x:c r="E16" s="31" t="str">
+      <x:c r="C16" s="52" t="str">
+        <x:v>S31660</x:v>
+      </x:c>
+      <x:c r="D16" s="52" t="str">
+        <x:v>Chan King</x:v>
+      </x:c>
+      <x:c r="E16" s="52" t="str">
         <x:v>Unit A</x:v>
       </x:c>
-      <x:c r="F16" s="31" t="str">
+      <x:c r="F16" s="52" t="str">
+        <x:v>General Staff 普通員工</x:v>
+      </x:c>
+      <x:c r="G16" s="52" t="str">
+        <x:v>HW2</x:v>
+      </x:c>
+      <x:c r="H16" s="52" t="str">
         <x:v>福利服務助理</x:v>
       </x:c>
-      <x:c r="G16" s="33" t="d">
-        <x:v>2018-03-08T00:00:00.0000000</x:v>
-      </x:c>
-      <x:c r="H16" s="31" t="n">
-        <x:v>2.041</x:v>
-      </x:c>
-      <x:c r="I16" s="31" t="str">
+      <x:c r="I16" s="54" t="d">
+        <x:v>2018-01-01T00:00:00.0000000</x:v>
+      </x:c>
+      <x:c r="J16" s="52" t="n">
+        <x:v>2.224</x:v>
+      </x:c>
+      <x:c r="K16" s="52" t="str">
         <x:v>AL14</x:v>
       </x:c>
-      <x:c r="J16" s="31" t="str">
+      <x:c r="L16" s="52" t="str">
         <x:v>Bank Holiday</x:v>
       </x:c>
-      <x:c r="K16" s="31" t="str">
+      <x:c r="M16" s="52" t="str">
         <x:v>Monthly</x:v>
       </x:c>
-      <x:c r="L16" s="31" t="n">
-        <x:v>20650</x:v>
-      </x:c>
-      <x:c r="M16" s="31" t="n">
-        <x:v>9</x:v>
-      </x:c>
-      <x:c r="N16" s="31" t="str">
-        <x:v>MPS</x:v>
-      </x:c>
-      <x:c r="O16" s="33" t="d">
-        <x:v>2018-03-08T00:00:00.0000000</x:v>
-      </x:c>
-      <x:c r="P16" s="33" t="d">
+      <x:c r="N16" s="52" t="n">
+        <x:v>16000</x:v>
+      </x:c>
+      <x:c r="O16" s="52" t="n">
+        <x:v>5</x:v>
+      </x:c>
+      <x:c r="P16" s="52" t="str">
+        <x:v/>
+      </x:c>
+      <x:c r="Q16" s="54" t="d">
+        <x:v>2018-12-14T00:00:00.0000000</x:v>
+      </x:c>
+      <x:c r="R16" s="54" t="d">
         <x:v>2045-01-01T00:00:00.0000000</x:v>
       </x:c>
-      <x:c r="Q16" s="31" t="str">
+      <x:c r="S16" s="52" t="str">
         <x:v>Active</x:v>
       </x:c>
-      <x:c r="R16" s="31" t="str">
+      <x:c r="T16" s="52" t="str">
         <x:v>No</x:v>
       </x:c>
-      <x:c r="S16" s="31" t="n">
+      <x:c r="U16" s="52" t="n">
         <x:v>39</x:v>
       </x:c>
-      <x:c r="T16" s="31" t="str">
+      <x:c r="V16" s="52" t="str">
         <x:v>DWS - CWB</x:v>
       </x:c>
     </x:row>
     <x:row r="17">
-      <x:c r="B17" s="31" t="str">
+      <x:c r="B17" s="52" t="str">
         <x:v>Data World Solutions Ltd</x:v>
       </x:c>
-      <x:c r="C17" s="31" t="str">
+      <x:c r="C17" s="52" t="str">
         <x:v>S31651</x:v>
       </x:c>
-      <x:c r="D17" s="31" t="str">
+      <x:c r="D17" s="52" t="str">
         <x:v>Chan Tai Man, Peter</x:v>
       </x:c>
-      <x:c r="E17" s="31" t="str">
+      <x:c r="E17" s="52" t="str">
         <x:v>Unit A</x:v>
       </x:c>
-      <x:c r="F17" s="31" t="str">
+      <x:c r="F17" s="52" t="str">
+        <x:v>General Staff 普通員工</x:v>
+      </x:c>
+      <x:c r="G17" s="52" t="str">
+        <x:v>PE</x:v>
+      </x:c>
+      <x:c r="H17" s="52" t="str">
         <x:v>Project Executive</x:v>
       </x:c>
-      <x:c r="G17" s="33" t="d">
+      <x:c r="I17" s="54" t="d">
         <x:v>2016-11-10T00:00:00.0000000</x:v>
       </x:c>
-      <x:c r="H17" s="31" t="n">
-        <x:v>3.3661</x:v>
-      </x:c>
-      <x:c r="I17" s="31" t="str">
+      <x:c r="J17" s="52" t="n">
+        <x:v>3.3689</x:v>
+      </x:c>
+      <x:c r="K17" s="52" t="str">
         <x:v>AL07</x:v>
       </x:c>
-      <x:c r="J17" s="31" t="str">
+      <x:c r="L17" s="52" t="str">
         <x:v>Bank Holiday</x:v>
       </x:c>
-      <x:c r="K17" s="31" t="str">
+      <x:c r="M17" s="52" t="str">
         <x:v>Monthly</x:v>
       </x:c>
-      <x:c r="L17" s="31" t="n">
+      <x:c r="N17" s="52" t="n">
         <x:v>30320</x:v>
       </x:c>
-      <x:c r="M17" s="31" t="n">
+      <x:c r="O17" s="52" t="n">
         <x:v>16</x:v>
       </x:c>
-      <x:c r="N17" s="31" t="str">
+      <x:c r="P17" s="52" t="str">
         <x:v>MPS</x:v>
       </x:c>
-      <x:c r="O17" s="33" t="d">
+      <x:c r="Q17" s="54" t="d">
         <x:v>2017-11-10T00:00:00.0000000</x:v>
       </x:c>
-      <x:c r="P17" s="33" t="d">
+      <x:c r="R17" s="54" t="d">
         <x:v>2045-01-01T00:00:00.0000000</x:v>
       </x:c>
-      <x:c r="Q17" s="31" t="str">
+      <x:c r="S17" s="52" t="str">
         <x:v>Active</x:v>
       </x:c>
-      <x:c r="R17" s="31" t="str">
+      <x:c r="T17" s="52" t="str">
         <x:v>No</x:v>
       </x:c>
-      <x:c r="S17" s="31" t="n">
+      <x:c r="U17" s="52" t="n">
         <x:v>39</x:v>
       </x:c>
-      <x:c r="T17" s="31" t="str">
-        <x:v>DWS - CWB</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="18">
-      <x:c r="B18" s="31" t="str">
-        <x:v>Data World Solutions Ltd</x:v>
-      </x:c>
-      <x:c r="C18" s="31" t="str">
-        <x:v>S31660</x:v>
-      </x:c>
-      <x:c r="D18" s="31" t="str">
-        <x:v>Chan King</x:v>
-      </x:c>
-      <x:c r="E18" s="31" t="str">
-        <x:v>Unit A</x:v>
-      </x:c>
-      <x:c r="F18" s="31" t="str">
-        <x:v>福利服務助理</x:v>
-      </x:c>
-      <x:c r="G18" s="33" t="d">
-        <x:v>2018-01-01T00:00:00.0000000</x:v>
-      </x:c>
-      <x:c r="H18" s="31" t="n">
-        <x:v>2.2213</x:v>
-      </x:c>
-      <x:c r="I18" s="31" t="str">
-        <x:v>AL14</x:v>
-      </x:c>
-      <x:c r="J18" s="31" t="str">
-        <x:v>Bank Holiday</x:v>
-      </x:c>
-      <x:c r="K18" s="31" t="str">
-        <x:v>Monthly</x:v>
-      </x:c>
-      <x:c r="L18" s="31" t="n">
-        <x:v>16000</x:v>
-      </x:c>
-      <x:c r="M18" s="31" t="n">
-        <x:v>5</x:v>
-      </x:c>
-      <x:c r="N18" s="31" t="str">
-        <x:v/>
-      </x:c>
-      <x:c r="O18" s="33" t="d">
-        <x:v>2018-12-14T00:00:00.0000000</x:v>
-      </x:c>
-      <x:c r="P18" s="33" t="d">
-        <x:v>2045-01-01T00:00:00.0000000</x:v>
-      </x:c>
-      <x:c r="Q18" s="31" t="str">
-        <x:v>Active</x:v>
-      </x:c>
-      <x:c r="R18" s="31" t="str">
-        <x:v>No</x:v>
-      </x:c>
-      <x:c r="S18" s="31" t="n">
-        <x:v>39</x:v>
-      </x:c>
-      <x:c r="T18" s="31" t="str">
+      <x:c r="V17" s="52" t="str">
         <x:v>DWS - CWB</x:v>
       </x:c>
     </x:row>
     <x:row r="19">
-      <x:c r="A19" s="31" t="str">
+      <x:c r="A19" s="52" t="str">
         <x:v>_DATAEND</x:v>
       </x:c>
-      <x:c r="B19" s="31" t="str">
-        <x:v>Data World Solutions Ltd</x:v>
-      </x:c>
-      <x:c r="C19" s="31" t="str">
-        <x:v>S31662</x:v>
-      </x:c>
-      <x:c r="D19" s="31" t="str">
-        <x:v>Chan Kit</x:v>
-      </x:c>
-      <x:c r="E19" s="31" t="str">
-        <x:v>Unit A</x:v>
-      </x:c>
-      <x:c r="F19" s="31" t="str">
-        <x:v>保健員</x:v>
-      </x:c>
-      <x:c r="G19" s="33" t="d">
-        <x:v>2019-01-01T00:00:00.0000000</x:v>
-      </x:c>
-      <x:c r="H19" s="31" t="n">
-        <x:v>1.2213</x:v>
-      </x:c>
-      <x:c r="I19" s="31" t="str">
-        <x:v>AL14</x:v>
-      </x:c>
-      <x:c r="J19" s="31" t="str">
-        <x:v>Bank Holiday</x:v>
-      </x:c>
-      <x:c r="K19" s="31" t="str">
-        <x:v>Monthly</x:v>
-      </x:c>
-      <x:c r="L19" s="31" t="n">
-        <x:v>15000</x:v>
-      </x:c>
-      <x:c r="M19" s="31" t="n">
-        <x:v>4</x:v>
-      </x:c>
-      <x:c r="N19" s="31" t="str">
-        <x:v/>
-      </x:c>
-      <x:c r="O19" s="33" t="d">
-        <x:v>2019-01-01T00:00:00.0000000</x:v>
-      </x:c>
-      <x:c r="P19" s="33" t="d">
-        <x:v>2045-01-01T00:00:00.0000000</x:v>
-      </x:c>
-      <x:c r="Q19" s="31" t="str">
-        <x:v>Active</x:v>
-      </x:c>
-      <x:c r="R19" s="31" t="str">
-        <x:v>No</x:v>
-      </x:c>
-      <x:c r="S19" s="31" t="n">
-        <x:v>39</x:v>
-      </x:c>
-      <x:c r="T19" s="31" t="str">
-        <x:v>DWS - CWB</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="21" spans="1:20" ht="16.5">
-      <x:c r="D21" s="4" t="s">
-        <x:v>83</x:v>
+      <x:c r="B19" s="53" t="str">
+        <x:v>Total</x:v>
+      </x:c>
+      <x:c r="J19" s="53" t="str">
+        <x:v>50.9887</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>